<commit_message>
posted final exam solutions and course gradelines
</commit_message>
<xml_diff>
--- a/418_S24/gradelines.xlsx
+++ b/418_S24/gradelines.xlsx
@@ -460,7 +460,7 @@
       </c>
       <c r="D2" s="2">
         <f>100*(SUM(E6:E15)/COUNT(E6:E15)*0.25 + SUM(E20:E22)*0.15 + E23*0.3)</f>
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -574,7 +574,7 @@
       </c>
       <c r="H10" s="8">
         <f>0.93*D16</f>
-        <v>148.8</v>
+        <v>167.4</v>
       </c>
       <c r="I10" s="8">
         <v>73.0</v>
@@ -585,10 +585,12 @@
       <c r="K10" s="6">
         <v>68.0</v>
       </c>
-      <c r="L10" s="8"/>
+      <c r="L10" s="8">
+        <v>95.0</v>
+      </c>
       <c r="M10" s="8">
         <f>IF(D16=0, 0, H10/D16)*H23 + IF(D20=0, 0, I10/D20)*I23 + IF(D21=0, 0, J10/D21)*J23 + IF(D22=0, 0, K10/D22)*K23 + IF(D23=0, 0, L10/D23)*L23</f>
-        <v>89.48076923</v>
+        <v>89.95535714</v>
       </c>
     </row>
     <row r="11">
@@ -607,7 +609,7 @@
       </c>
       <c r="H11" s="8">
         <f>0.9*D16</f>
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="I11" s="8">
         <v>68.0</v>
@@ -618,10 +620,12 @@
       <c r="K11" s="6">
         <v>61.0</v>
       </c>
-      <c r="L11" s="8"/>
+      <c r="L11" s="8">
+        <v>86.0</v>
+      </c>
       <c r="M11" s="8">
         <f>IF(D16=0, 0, H11/D16)*H23 + IF(D20=0, 0, I11/D20)*I23 + IF(D21=0, 0, J11/D21)*J23 + IF(D22=0, 0, K11/D22)*K23 + IF(D23=0, 0, L11/D23)*L23</f>
-        <v>83.17307692</v>
+        <v>83.13392857</v>
       </c>
     </row>
     <row r="12">
@@ -640,7 +644,7 @@
       </c>
       <c r="H12" s="8">
         <f>0.87*D16</f>
-        <v>139.2</v>
+        <v>156.6</v>
       </c>
       <c r="I12" s="8">
         <v>63.0</v>
@@ -651,10 +655,12 @@
       <c r="K12" s="6">
         <v>53.0</v>
       </c>
-      <c r="L12" s="8"/>
+      <c r="L12" s="8">
+        <v>78.0</v>
+      </c>
       <c r="M12" s="8">
         <f>IF(D16=0, 0, H12/D16)*H23 + IF(D20=0, 0, I12/D20)*I23 + IF(D21=0, 0, J12/D21)*J23 + IF(D22=0, 0, K12/D22)*K23 + IF(D23=0, 0, L12/D23)*L23</f>
-        <v>76.8974359</v>
+        <v>76.61904762</v>
       </c>
     </row>
     <row r="13">
@@ -673,7 +679,7 @@
       </c>
       <c r="H13" s="8">
         <f>0.83*D16</f>
-        <v>132.8</v>
+        <v>149.4</v>
       </c>
       <c r="I13" s="8">
         <v>57.0</v>
@@ -684,10 +690,12 @@
       <c r="K13" s="6">
         <v>46.0</v>
       </c>
-      <c r="L13" s="8"/>
+      <c r="L13" s="8">
+        <v>71.0</v>
+      </c>
       <c r="M13" s="8">
         <f>IF(D16=0, 0, H13/D16)*H23 + IF(D20=0, 0, I13/D20)*I23 + IF(D21=0, 0, J13/D21)*J23 + IF(D22=0, 0, K13/D22)*K23 + IF(D23=0, 0, L13/D23)*L23</f>
-        <v>70.31410256</v>
+        <v>70.13988095</v>
       </c>
     </row>
     <row r="14">
@@ -699,14 +707,14 @@
         <v>20.0</v>
       </c>
       <c r="E14" s="6">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>31</v>
       </c>
       <c r="H14" s="8">
         <f>0.8*D16</f>
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="I14" s="8">
         <v>50.0</v>
@@ -717,10 +725,12 @@
       <c r="K14" s="6">
         <v>39.0</v>
       </c>
-      <c r="L14" s="8"/>
+      <c r="L14" s="8">
+        <v>64.0</v>
+      </c>
       <c r="M14" s="8">
         <f>IF(D16=0, 0, H14/D16)*H23 + IF(D20=0, 0, I14/D20)*I23 + IF(D21=0, 0, J14/D21)*J23 + IF(D22=0, 0, K14/D22)*K23 + IF(D23=0, 0, L14/D23)*L23</f>
-        <v>63.75</v>
+        <v>63.72321429</v>
       </c>
     </row>
     <row r="15">
@@ -732,14 +742,14 @@
         <v>20.0</v>
       </c>
       <c r="E15" s="6">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>33</v>
       </c>
       <c r="H15" s="8">
         <f>0.77*D16</f>
-        <v>123.2</v>
+        <v>138.6</v>
       </c>
       <c r="I15" s="8">
         <v>44.0</v>
@@ -750,10 +760,12 @@
       <c r="K15" s="6">
         <v>32.0</v>
       </c>
-      <c r="L15" s="8"/>
+      <c r="L15" s="8">
+        <v>56.0</v>
+      </c>
       <c r="M15" s="8">
         <f>IF(D16=0, 0, H15/D16)*H23 + IF(D20=0, 0, I15/D20)*I23 + IF(D21=0, 0, J15/D21)*J23 + IF(D22=0, 0, K15/D22)*K23 + IF(D23=0, 0, L15/D23)*L23</f>
-        <v>57.47435897</v>
+        <v>57.20833333</v>
       </c>
     </row>
     <row r="16">
@@ -766,7 +778,7 @@
       </c>
       <c r="D16" s="6">
         <f>20*MIN(SUM(E6:E15),COUNT(E6:E15)-1)</f>
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="E16" s="6"/>
       <c r="G16" s="7" t="s">
@@ -774,7 +786,7 @@
       </c>
       <c r="H16" s="8">
         <f>0.73*D16</f>
-        <v>116.8</v>
+        <v>131.4</v>
       </c>
       <c r="I16" s="8">
         <v>37.0</v>
@@ -785,10 +797,12 @@
       <c r="K16" s="6">
         <v>27.0</v>
       </c>
-      <c r="L16" s="8"/>
+      <c r="L16" s="8">
+        <v>48.0</v>
+      </c>
       <c r="M16" s="8">
         <f>IF(D16=0, 0, H16/D16)*H23 + IF(D20=0, 0, I16/D20)*I23 + IF(D21=0, 0, J16/D21)*J23 + IF(D22=0, 0, K16/D22)*K23 + IF(D23=0, 0, L16/D23)*L23</f>
-        <v>50.53846154</v>
+        <v>50.21428571</v>
       </c>
     </row>
     <row r="17">
@@ -797,7 +811,7 @@
       </c>
       <c r="H17" s="8">
         <f>0.7*D16</f>
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="I17" s="8">
         <v>30.0</v>
@@ -808,10 +822,12 @@
       <c r="K17" s="6">
         <v>18.0</v>
       </c>
-      <c r="L17" s="8"/>
+      <c r="L17" s="8">
+        <v>40.0</v>
+      </c>
       <c r="M17" s="8">
         <f>IF(D16=0, 0, H17/D16)*H23 + IF(D20=0, 0, I17/D20)*I23 + IF(D21=0, 0, J17/D21)*J23 + IF(D22=0, 0, K17/D22)*K23 + IF(D23=0, 0, L17/D23)*L23</f>
-        <v>42.43589744</v>
+        <v>42.51190476</v>
       </c>
     </row>
     <row r="18">
@@ -820,7 +836,7 @@
       </c>
       <c r="H18" s="8">
         <f>0.67*D16</f>
-        <v>107.2</v>
+        <v>120.6</v>
       </c>
       <c r="I18" s="8">
         <v>24.0</v>
@@ -831,10 +847,12 @@
       <c r="K18" s="6">
         <v>12.0</v>
       </c>
-      <c r="L18" s="8"/>
+      <c r="L18" s="8">
+        <v>30.0</v>
+      </c>
       <c r="M18" s="8">
         <f>IF(D16=0, 0, H18/D16)*H23 + IF(D20=0, 0, I18/D20)*I23 + IF(D21=0, 0, J18/D21)*J23 + IF(D22=0, 0, K18/D22)*K23 + IF(D23=0, 0, L18/D23)*L23</f>
-        <v>36.44871795</v>
+        <v>35.61309524</v>
       </c>
     </row>
     <row r="19">
@@ -855,7 +873,7 @@
       </c>
       <c r="H19" s="8">
         <f>0.63*D16</f>
-        <v>100.8</v>
+        <v>113.4</v>
       </c>
       <c r="I19" s="8">
         <v>18.0</v>
@@ -866,10 +884,12 @@
       <c r="K19" s="6">
         <v>8.0</v>
       </c>
-      <c r="L19" s="8"/>
+      <c r="L19" s="8">
+        <v>20.0</v>
+      </c>
       <c r="M19" s="8">
         <f>IF(D16=0, 0, H19/D16)*H23 + IF(D20=0, 0, I19/D20)*I23 + IF(D21=0, 0, J19/D21)*J23 + IF(D22=0, 0, K19/D22)*K23 + IF(D23=0, 0, L19/D23)*L23</f>
-        <v>31.05128205</v>
+        <v>29.04761905</v>
       </c>
     </row>
     <row r="20">
@@ -888,7 +908,7 @@
       </c>
       <c r="H20" s="8">
         <f>0.6*D16</f>
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="I20" s="8">
         <v>13.0</v>
@@ -899,10 +919,12 @@
       <c r="K20" s="6">
         <v>5.0</v>
       </c>
-      <c r="L20" s="8"/>
+      <c r="L20" s="8">
+        <v>10.0</v>
+      </c>
       <c r="M20" s="8">
         <f>IF(D16=0, 0, H20/D16)*H23 + IF(D20=0, 0, I20/D20)*I23 + IF(D21=0, 0, J20/D21)*J23 + IF(D22=0, 0, K20/D22)*K23 + IF(D23=0, 0, L20/D23)*L23</f>
-        <v>26.53846154</v>
+        <v>23.10714286</v>
       </c>
     </row>
     <row r="21">
@@ -932,7 +954,9 @@
       <c r="K21" s="6">
         <v>0.0</v>
       </c>
-      <c r="L21" s="8"/>
+      <c r="L21" s="8">
+        <v>0.0</v>
+      </c>
       <c r="M21" s="8">
         <f>IF(D16=0, 0, H21/D16)*H23 + IF(D20=0, 0, I21/D20)*I23 + IF(D21=0, 0, J21/D21)*J23 + IF(D22=0, 0, K21/D22)*K23 + IF(D23=0, 0, L21/D23)*L23</f>
         <v>0</v>
@@ -983,33 +1007,33 @@
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="7">
-        <v>72.0</v>
+        <v>105.0</v>
       </c>
       <c r="E23" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>42</v>
       </c>
       <c r="H23" s="8">
         <f>10000*(SUM(E6:E15)/COUNT(E6:E15)*0.25) / D2</f>
-        <v>30.76923077</v>
+        <v>25</v>
       </c>
       <c r="I23" s="8">
         <f>10000*E20*0.15 / D2</f>
-        <v>23.07692308</v>
+        <v>15</v>
       </c>
       <c r="J23" s="8">
         <f>10000*E21*0.15 / D2</f>
-        <v>23.07692308</v>
+        <v>15</v>
       </c>
       <c r="K23" s="8">
         <f>10000*E22*0.15 / D2</f>
-        <v>23.07692308</v>
+        <v>15</v>
       </c>
       <c r="L23" s="8">
         <f>10000*E23*0.3 / D2</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M23" s="8">
         <f>SUM(H23:L23)</f>

</xml_diff>